<commit_message>
Refactorización y reestructuración de carpetas de documentación
</commit_message>
<xml_diff>
--- a/docs/DiagramaGantt.xlsx
+++ b/docs/DiagramaGantt.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECCB72E-E205-4850-B775-BC2EADDEE999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59645F1E-607D-41D2-BC40-9A75922614A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="61">
   <si>
     <t>SOBRE ESTE DIAGRAMA DE GANTT</t>
   </si>
@@ -841,7 +841,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1219,15 +1219,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="2" tint="-0.14999847407452621"/>
       </left>
@@ -1284,19 +1275,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </left>
       <right/>
@@ -1329,21 +1307,6 @@
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.14999847407452621"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1413,7 +1376,7 @@
     <xf numFmtId="0" fontId="4" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1766,15 +1729,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="13" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1808,13 +1762,13 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1898,6 +1852,92 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="55">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2192,92 +2232,6 @@
         <bottom style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2816,8 +2770,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Hitos4352" displayName="Hitos4352" ref="B9:F38" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="B9:F38" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Hitos4352" displayName="Hitos4352" ref="B9:F34" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="B9:F34" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3180,11 +3134,11 @@
     <row r="2" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="7"/>
       <c r="B2" s="96"/>
-      <c r="C2" s="133" t="s">
+      <c r="C2" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="96"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -3212,11 +3166,11 @@
     <row r="4" spans="1:13" s="8" customFormat="1" ht="67.2" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="7"/>
       <c r="B4" s="91"/>
-      <c r="C4" s="134" t="s">
+      <c r="C4" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
       <c r="F4" s="91"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -3229,11 +3183,11 @@
     <row r="5" spans="1:13" s="8" customFormat="1" ht="67.2" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="7"/>
       <c r="B5" s="91"/>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
       <c r="F5" s="91"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -3333,10 +3287,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO39"/>
+  <dimension ref="A1:BO36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A6" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AK20" sqref="AK20"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="BJ6" sqref="BJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3354,26 +3308,26 @@
     <row r="1" spans="1:67" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:67" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="135" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="139"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="139"/>
-      <c r="L2" s="139"/>
-      <c r="M2" s="139"/>
-      <c r="N2" s="140"/>
-      <c r="O2" s="140"/>
-      <c r="P2" s="140"/>
-      <c r="Q2" s="140"/>
-      <c r="R2" s="140"/>
-      <c r="S2" s="140"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="137"/>
+      <c r="O2" s="137"/>
+      <c r="P2" s="137"/>
+      <c r="Q2" s="137"/>
+      <c r="R2" s="137"/>
+      <c r="S2" s="137"/>
       <c r="T2" s="60"/>
       <c r="U2" s="60"/>
       <c r="V2" s="60"/>
@@ -3445,36 +3399,36 @@
         <v>30</v>
       </c>
       <c r="G4" s="68"/>
-      <c r="H4" s="141" t="s">
+      <c r="H4" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="M4" s="142" t="s">
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="M4" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="142"/>
-      <c r="O4" s="142"/>
-      <c r="P4" s="142"/>
-      <c r="R4" s="143" t="s">
+      <c r="N4" s="139"/>
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="R4" s="140" t="s">
         <v>23</v>
       </c>
-      <c r="S4" s="143"/>
-      <c r="T4" s="143"/>
-      <c r="U4" s="143"/>
-      <c r="W4" s="147" t="s">
+      <c r="S4" s="140"/>
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
+      <c r="W4" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="X4" s="147"/>
-      <c r="Y4" s="147"/>
-      <c r="Z4" s="147"/>
-      <c r="AB4" s="148" t="s">
+      <c r="X4" s="144"/>
+      <c r="Y4" s="144"/>
+      <c r="Z4" s="144"/>
+      <c r="AB4" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="AC4" s="148"/>
-      <c r="AD4" s="148"/>
-      <c r="AE4" s="148"/>
+      <c r="AC4" s="145"/>
+      <c r="AD4" s="145"/>
+      <c r="AE4" s="145"/>
     </row>
     <row r="5" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
@@ -3493,7 +3447,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="73">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="69"/>
@@ -3594,227 +3548,227 @@
       <c r="G7" s="75"/>
       <c r="H7" s="107">
         <f ca="1">IFERROR(Inicio_del_proyecto+Incremento_de_desplazamiento,TODAY())</f>
-        <v>45752</v>
+        <v>45755</v>
       </c>
       <c r="I7" s="108">
         <f ca="1">H7+1</f>
-        <v>45753</v>
+        <v>45756</v>
       </c>
       <c r="J7" s="108">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>45754</v>
+        <v>45757</v>
       </c>
       <c r="K7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45755</v>
+        <v>45758</v>
       </c>
       <c r="L7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45756</v>
+        <v>45759</v>
       </c>
       <c r="M7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45757</v>
+        <v>45760</v>
       </c>
       <c r="N7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45758</v>
+        <v>45761</v>
       </c>
       <c r="O7" s="108">
         <f ca="1">N7+1</f>
-        <v>45759</v>
+        <v>45762</v>
       </c>
       <c r="P7" s="108">
         <f ca="1">O7+1</f>
-        <v>45760</v>
+        <v>45763</v>
       </c>
       <c r="Q7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45761</v>
+        <v>45764</v>
       </c>
       <c r="R7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45762</v>
+        <v>45765</v>
       </c>
       <c r="S7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45763</v>
+        <v>45766</v>
       </c>
       <c r="T7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45764</v>
+        <v>45767</v>
       </c>
       <c r="U7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45765</v>
+        <v>45768</v>
       </c>
       <c r="V7" s="108">
         <f ca="1">U7+1</f>
-        <v>45766</v>
+        <v>45769</v>
       </c>
       <c r="W7" s="108">
         <f ca="1">V7+1</f>
-        <v>45767</v>
+        <v>45770</v>
       </c>
       <c r="X7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45768</v>
+        <v>45771</v>
       </c>
       <c r="Y7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45769</v>
+        <v>45772</v>
       </c>
       <c r="Z7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="AA7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45771</v>
+        <v>45774</v>
       </c>
       <c r="AB7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45772</v>
+        <v>45775</v>
       </c>
       <c r="AC7" s="108">
         <f ca="1">AB7+1</f>
-        <v>45773</v>
+        <v>45776</v>
       </c>
       <c r="AD7" s="108">
         <f ca="1">AC7+1</f>
-        <v>45774</v>
+        <v>45777</v>
       </c>
       <c r="AE7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45775</v>
+        <v>45778</v>
       </c>
       <c r="AF7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="AG7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45777</v>
+        <v>45780</v>
       </c>
       <c r="AH7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45778</v>
+        <v>45781</v>
       </c>
       <c r="AI7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45779</v>
+        <v>45782</v>
       </c>
       <c r="AJ7" s="108">
         <f ca="1">AI7+1</f>
-        <v>45780</v>
+        <v>45783</v>
       </c>
       <c r="AK7" s="108">
         <f ca="1">AJ7+1</f>
-        <v>45781</v>
+        <v>45784</v>
       </c>
       <c r="AL7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45782</v>
+        <v>45785</v>
       </c>
       <c r="AM7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45783</v>
+        <v>45786</v>
       </c>
       <c r="AN7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45784</v>
+        <v>45787</v>
       </c>
       <c r="AO7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45785</v>
+        <v>45788</v>
       </c>
       <c r="AP7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45786</v>
+        <v>45789</v>
       </c>
       <c r="AQ7" s="108">
         <f ca="1">AP7+1</f>
-        <v>45787</v>
+        <v>45790</v>
       </c>
       <c r="AR7" s="108">
         <f ca="1">AQ7+1</f>
-        <v>45788</v>
+        <v>45791</v>
       </c>
       <c r="AS7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45789</v>
+        <v>45792</v>
       </c>
       <c r="AT7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45790</v>
+        <v>45793</v>
       </c>
       <c r="AU7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45791</v>
+        <v>45794</v>
       </c>
       <c r="AV7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45792</v>
+        <v>45795</v>
       </c>
       <c r="AW7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45793</v>
+        <v>45796</v>
       </c>
       <c r="AX7" s="108">
         <f ca="1">AW7+1</f>
-        <v>45794</v>
+        <v>45797</v>
       </c>
       <c r="AY7" s="108">
         <f ca="1">AX7+1</f>
-        <v>45795</v>
+        <v>45798</v>
       </c>
       <c r="AZ7" s="108">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>45796</v>
+        <v>45799</v>
       </c>
       <c r="BA7" s="108">
         <f t="shared" ca="1" si="1"/>
-        <v>45797</v>
+        <v>45800</v>
       </c>
       <c r="BB7" s="108">
         <f t="shared" ca="1" si="1"/>
-        <v>45798</v>
+        <v>45801</v>
       </c>
       <c r="BC7" s="108">
         <f t="shared" ca="1" si="1"/>
-        <v>45799</v>
+        <v>45802</v>
       </c>
       <c r="BD7" s="109">
         <f t="shared" ca="1" si="1"/>
-        <v>45800</v>
+        <v>45803</v>
       </c>
       <c r="BE7" s="108">
         <f ca="1">BD7+1</f>
-        <v>45801</v>
+        <v>45804</v>
       </c>
       <c r="BF7" s="108">
         <f ca="1">BE7+1</f>
-        <v>45802</v>
+        <v>45805</v>
       </c>
       <c r="BG7" s="108">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>45803</v>
+        <v>45806</v>
       </c>
       <c r="BH7" s="108">
         <f t="shared" ca="1" si="2"/>
-        <v>45804</v>
+        <v>45807</v>
       </c>
       <c r="BI7" s="108">
         <f t="shared" ca="1" si="2"/>
-        <v>45805</v>
+        <v>45808</v>
       </c>
       <c r="BJ7" s="108">
         <f t="shared" ca="1" si="2"/>
-        <v>45806</v>
+        <v>45809</v>
       </c>
       <c r="BK7" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>45807</v>
+        <v>45810</v>
       </c>
     </row>
     <row r="8" spans="1:67" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3902,227 +3856,227 @@
       <c r="G9" s="80"/>
       <c r="H9" s="89" t="str">
         <f t="shared" ref="H9:BK9" ca="1" si="3">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="I9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="J9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>j</v>
       </c>
       <c r="K9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="L9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="M9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>d</v>
       </c>
       <c r="N9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>l</v>
       </c>
       <c r="O9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="P9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="Q9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>j</v>
       </c>
       <c r="R9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="S9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="T9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>d</v>
       </c>
       <c r="U9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>l</v>
       </c>
       <c r="V9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="W9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="X9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>j</v>
       </c>
       <c r="Y9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="Z9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AA9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>d</v>
       </c>
       <c r="AB9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>l</v>
       </c>
       <c r="AC9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AD9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="AE9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>j</v>
       </c>
       <c r="AF9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="AG9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AH9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>d</v>
       </c>
       <c r="AI9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>l</v>
       </c>
       <c r="AJ9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AK9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="AL9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>j</v>
       </c>
       <c r="AM9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="AN9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AO9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>d</v>
       </c>
       <c r="AP9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>l</v>
       </c>
       <c r="AQ9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AR9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="AS9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>j</v>
       </c>
       <c r="AT9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="AU9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AV9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>d</v>
       </c>
       <c r="AW9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>l</v>
       </c>
       <c r="AX9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AY9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="AZ9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>j</v>
       </c>
       <c r="BA9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="BB9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="BC9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>d</v>
       </c>
       <c r="BD9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>l</v>
       </c>
       <c r="BE9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="BF9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="BG9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>j</v>
       </c>
       <c r="BH9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="BI9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="BJ9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>d</v>
       </c>
       <c r="BK9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>l</v>
       </c>
     </row>
     <row r="10" spans="1:67" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4198,65 +4152,65 @@
       <c r="E11" s="55"/>
       <c r="F11" s="56"/>
       <c r="G11" s="53"/>
-      <c r="H11" s="135" t="str">
+      <c r="H11" s="132" t="str">
         <f t="shared" ref="H11:H19" ca="1" si="4">IF(AND($C11="Objetivo",H$7&gt;=$E11,H$7&lt;=$E11+$F11-1),2,IF(AND($C11="Hito",H$7&gt;=$E11,H$7&lt;=$E11+$F11-1),1,""))</f>
         <v/>
       </c>
-      <c r="I11" s="136"/>
-      <c r="J11" s="136"/>
-      <c r="K11" s="136"/>
-      <c r="L11" s="136"/>
-      <c r="M11" s="136"/>
-      <c r="N11" s="136"/>
-      <c r="O11" s="136"/>
-      <c r="P11" s="136"/>
-      <c r="Q11" s="136"/>
-      <c r="R11" s="136"/>
-      <c r="S11" s="136"/>
-      <c r="T11" s="136"/>
-      <c r="U11" s="136"/>
-      <c r="V11" s="136"/>
-      <c r="W11" s="136"/>
-      <c r="X11" s="136"/>
-      <c r="Y11" s="136"/>
-      <c r="Z11" s="136"/>
-      <c r="AA11" s="136"/>
-      <c r="AB11" s="136"/>
-      <c r="AC11" s="136"/>
-      <c r="AD11" s="136"/>
-      <c r="AE11" s="136"/>
-      <c r="AF11" s="136"/>
-      <c r="AG11" s="136"/>
-      <c r="AH11" s="136"/>
-      <c r="AI11" s="136"/>
-      <c r="AJ11" s="136"/>
-      <c r="AK11" s="136"/>
-      <c r="AL11" s="136"/>
-      <c r="AM11" s="136"/>
-      <c r="AN11" s="136"/>
-      <c r="AO11" s="136"/>
-      <c r="AP11" s="136"/>
-      <c r="AQ11" s="136"/>
-      <c r="AR11" s="136"/>
-      <c r="AS11" s="136"/>
-      <c r="AT11" s="136"/>
-      <c r="AU11" s="136"/>
-      <c r="AV11" s="136"/>
-      <c r="AW11" s="136"/>
-      <c r="AX11" s="136"/>
-      <c r="AY11" s="136"/>
-      <c r="AZ11" s="136"/>
-      <c r="BA11" s="136"/>
-      <c r="BB11" s="136"/>
-      <c r="BC11" s="136"/>
-      <c r="BD11" s="136"/>
-      <c r="BE11" s="136"/>
-      <c r="BF11" s="136"/>
-      <c r="BG11" s="136"/>
-      <c r="BH11" s="136"/>
-      <c r="BI11" s="136"/>
-      <c r="BJ11" s="136"/>
-      <c r="BK11" s="137"/>
+      <c r="I11" s="133"/>
+      <c r="J11" s="133"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="133"/>
+      <c r="M11" s="133"/>
+      <c r="N11" s="133"/>
+      <c r="O11" s="133"/>
+      <c r="P11" s="133"/>
+      <c r="Q11" s="133"/>
+      <c r="R11" s="133"/>
+      <c r="S11" s="133"/>
+      <c r="T11" s="133"/>
+      <c r="U11" s="133"/>
+      <c r="V11" s="133"/>
+      <c r="W11" s="133"/>
+      <c r="X11" s="133"/>
+      <c r="Y11" s="133"/>
+      <c r="Z11" s="133"/>
+      <c r="AA11" s="133"/>
+      <c r="AB11" s="133"/>
+      <c r="AC11" s="133"/>
+      <c r="AD11" s="133"/>
+      <c r="AE11" s="133"/>
+      <c r="AF11" s="133"/>
+      <c r="AG11" s="133"/>
+      <c r="AH11" s="133"/>
+      <c r="AI11" s="133"/>
+      <c r="AJ11" s="133"/>
+      <c r="AK11" s="133"/>
+      <c r="AL11" s="133"/>
+      <c r="AM11" s="133"/>
+      <c r="AN11" s="133"/>
+      <c r="AO11" s="133"/>
+      <c r="AP11" s="133"/>
+      <c r="AQ11" s="133"/>
+      <c r="AR11" s="133"/>
+      <c r="AS11" s="133"/>
+      <c r="AT11" s="133"/>
+      <c r="AU11" s="133"/>
+      <c r="AV11" s="133"/>
+      <c r="AW11" s="133"/>
+      <c r="AX11" s="133"/>
+      <c r="AY11" s="133"/>
+      <c r="AZ11" s="133"/>
+      <c r="BA11" s="133"/>
+      <c r="BB11" s="133"/>
+      <c r="BC11" s="133"/>
+      <c r="BD11" s="133"/>
+      <c r="BE11" s="133"/>
+      <c r="BF11" s="133"/>
+      <c r="BG11" s="133"/>
+      <c r="BH11" s="133"/>
+      <c r="BI11" s="133"/>
+      <c r="BJ11" s="133"/>
+      <c r="BK11" s="134"/>
       <c r="BO11" s="36"/>
     </row>
     <row r="12" spans="1:67" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -4998,62 +4952,62 @@
       <c r="E15" s="55"/>
       <c r="F15" s="56"/>
       <c r="G15" s="53"/>
-      <c r="H15" s="135"/>
-      <c r="I15" s="136"/>
-      <c r="J15" s="136"/>
-      <c r="K15" s="136"/>
-      <c r="L15" s="136"/>
-      <c r="M15" s="136"/>
-      <c r="N15" s="136"/>
-      <c r="O15" s="136"/>
-      <c r="P15" s="136"/>
-      <c r="Q15" s="136"/>
-      <c r="R15" s="136"/>
-      <c r="S15" s="136"/>
-      <c r="T15" s="136"/>
-      <c r="U15" s="136"/>
-      <c r="V15" s="136"/>
-      <c r="W15" s="136"/>
-      <c r="X15" s="136"/>
-      <c r="Y15" s="136"/>
-      <c r="Z15" s="136"/>
-      <c r="AA15" s="136"/>
-      <c r="AB15" s="136"/>
-      <c r="AC15" s="136"/>
-      <c r="AD15" s="136"/>
-      <c r="AE15" s="136"/>
-      <c r="AF15" s="136"/>
-      <c r="AG15" s="136"/>
-      <c r="AH15" s="136"/>
-      <c r="AI15" s="136"/>
-      <c r="AJ15" s="136"/>
-      <c r="AK15" s="136"/>
-      <c r="AL15" s="136"/>
-      <c r="AM15" s="136"/>
-      <c r="AN15" s="136"/>
-      <c r="AO15" s="136"/>
-      <c r="AP15" s="136"/>
-      <c r="AQ15" s="136"/>
-      <c r="AR15" s="136"/>
-      <c r="AS15" s="136"/>
-      <c r="AT15" s="136"/>
-      <c r="AU15" s="136"/>
-      <c r="AV15" s="136"/>
-      <c r="AW15" s="136"/>
-      <c r="AX15" s="136"/>
-      <c r="AY15" s="136"/>
-      <c r="AZ15" s="136"/>
-      <c r="BA15" s="136"/>
-      <c r="BB15" s="136"/>
-      <c r="BC15" s="136"/>
-      <c r="BD15" s="136"/>
-      <c r="BE15" s="136"/>
-      <c r="BF15" s="136"/>
-      <c r="BG15" s="136"/>
-      <c r="BH15" s="136"/>
-      <c r="BI15" s="136"/>
-      <c r="BJ15" s="136"/>
-      <c r="BK15" s="137"/>
+      <c r="H15" s="132"/>
+      <c r="I15" s="133"/>
+      <c r="J15" s="133"/>
+      <c r="K15" s="133"/>
+      <c r="L15" s="133"/>
+      <c r="M15" s="133"/>
+      <c r="N15" s="133"/>
+      <c r="O15" s="133"/>
+      <c r="P15" s="133"/>
+      <c r="Q15" s="133"/>
+      <c r="R15" s="133"/>
+      <c r="S15" s="133"/>
+      <c r="T15" s="133"/>
+      <c r="U15" s="133"/>
+      <c r="V15" s="133"/>
+      <c r="W15" s="133"/>
+      <c r="X15" s="133"/>
+      <c r="Y15" s="133"/>
+      <c r="Z15" s="133"/>
+      <c r="AA15" s="133"/>
+      <c r="AB15" s="133"/>
+      <c r="AC15" s="133"/>
+      <c r="AD15" s="133"/>
+      <c r="AE15" s="133"/>
+      <c r="AF15" s="133"/>
+      <c r="AG15" s="133"/>
+      <c r="AH15" s="133"/>
+      <c r="AI15" s="133"/>
+      <c r="AJ15" s="133"/>
+      <c r="AK15" s="133"/>
+      <c r="AL15" s="133"/>
+      <c r="AM15" s="133"/>
+      <c r="AN15" s="133"/>
+      <c r="AO15" s="133"/>
+      <c r="AP15" s="133"/>
+      <c r="AQ15" s="133"/>
+      <c r="AR15" s="133"/>
+      <c r="AS15" s="133"/>
+      <c r="AT15" s="133"/>
+      <c r="AU15" s="133"/>
+      <c r="AV15" s="133"/>
+      <c r="AW15" s="133"/>
+      <c r="AX15" s="133"/>
+      <c r="AY15" s="133"/>
+      <c r="AZ15" s="133"/>
+      <c r="BA15" s="133"/>
+      <c r="BB15" s="133"/>
+      <c r="BC15" s="133"/>
+      <c r="BD15" s="133"/>
+      <c r="BE15" s="133"/>
+      <c r="BF15" s="133"/>
+      <c r="BG15" s="133"/>
+      <c r="BH15" s="133"/>
+      <c r="BI15" s="133"/>
+      <c r="BJ15" s="133"/>
+      <c r="BK15" s="134"/>
     </row>
     <row r="16" spans="1:67" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
@@ -5158,7 +5112,7 @@
         <v/>
       </c>
       <c r="AC16" s="24" t="str">
-        <f t="shared" ref="AC16:AL19" ca="1" si="12">IF(AND($C16="Objetivo",AC$7&gt;=$E16,AC$7&lt;=$E16+$F16-1),2,IF(AND($C16="Hito",AC$7&gt;=$E16,AC$7&lt;=$E16+$F16-1),1,""))</f>
+        <f t="shared" ref="AC16:AL20" ca="1" si="12">IF(AND($C16="Objetivo",AC$7&gt;=$E16,AC$7&lt;=$E16+$F16-1),2,IF(AND($C16="Hito",AC$7&gt;=$E16,AC$7&lt;=$E16+$F16-1),1,""))</f>
         <v/>
       </c>
       <c r="AD16" s="24" t="str">
@@ -6050,62 +6004,62 @@
         <v>1</v>
       </c>
       <c r="G20" s="53"/>
-      <c r="H20" s="126"/>
-      <c r="I20" s="126"/>
-      <c r="J20" s="127"/>
-      <c r="K20" s="126"/>
-      <c r="L20" s="128"/>
-      <c r="M20" s="127"/>
-      <c r="N20" s="129"/>
-      <c r="O20" s="130"/>
-      <c r="P20" s="127"/>
-      <c r="Q20" s="130"/>
-      <c r="R20" s="127"/>
-      <c r="S20" s="130"/>
-      <c r="T20" s="127"/>
-      <c r="U20" s="127"/>
-      <c r="V20" s="130"/>
-      <c r="W20" s="127"/>
-      <c r="X20" s="126"/>
+      <c r="H20" s="125"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="126"/>
+      <c r="K20" s="125"/>
+      <c r="L20" s="127"/>
+      <c r="M20" s="126"/>
+      <c r="N20" s="128"/>
+      <c r="O20" s="129"/>
+      <c r="P20" s="126"/>
+      <c r="Q20" s="129"/>
+      <c r="R20" s="126"/>
+      <c r="S20" s="129"/>
+      <c r="T20" s="126"/>
+      <c r="U20" s="126"/>
+      <c r="V20" s="129"/>
+      <c r="W20" s="126"/>
+      <c r="X20" s="125"/>
       <c r="Y20" s="124"/>
-      <c r="Z20" s="127"/>
-      <c r="AA20" s="129"/>
-      <c r="AB20" s="126"/>
-      <c r="AC20" s="127"/>
-      <c r="AD20" s="127"/>
-      <c r="AE20" s="129"/>
+      <c r="Z20" s="126"/>
+      <c r="AA20" s="128"/>
+      <c r="AB20" s="125"/>
+      <c r="AC20" s="126"/>
+      <c r="AD20" s="126"/>
+      <c r="AE20" s="128"/>
       <c r="AF20" s="124"/>
       <c r="AG20" s="124"/>
       <c r="AH20" s="124"/>
-      <c r="AI20" s="130"/>
-      <c r="AJ20" s="127"/>
-      <c r="AK20" s="132"/>
-      <c r="AL20" s="125"/>
-      <c r="AM20" s="127"/>
-      <c r="AN20" s="125"/>
-      <c r="AO20" s="131"/>
-      <c r="AP20" s="125"/>
-      <c r="AQ20" s="126"/>
-      <c r="AR20" s="127"/>
-      <c r="AS20" s="127"/>
-      <c r="AT20" s="127"/>
-      <c r="AU20" s="129"/>
-      <c r="AV20" s="130"/>
-      <c r="AW20" s="127"/>
-      <c r="AX20" s="129"/>
-      <c r="AY20" s="130"/>
-      <c r="AZ20" s="127"/>
-      <c r="BA20" s="126"/>
-      <c r="BB20" s="126"/>
-      <c r="BC20" s="127"/>
-      <c r="BD20" s="127"/>
-      <c r="BE20" s="126"/>
-      <c r="BF20" s="127"/>
-      <c r="BG20" s="129"/>
-      <c r="BH20" s="130"/>
-      <c r="BI20" s="127"/>
-      <c r="BJ20" s="127"/>
-      <c r="BK20" s="129"/>
+      <c r="AI20" s="129"/>
+      <c r="AJ20" s="126"/>
+      <c r="AK20" s="126"/>
+      <c r="AL20" s="126"/>
+      <c r="AM20" s="126"/>
+      <c r="AN20" s="126"/>
+      <c r="AO20" s="126"/>
+      <c r="AP20" s="126"/>
+      <c r="AQ20" s="125"/>
+      <c r="AR20" s="126"/>
+      <c r="AS20" s="126"/>
+      <c r="AT20" s="126"/>
+      <c r="AU20" s="128"/>
+      <c r="AV20" s="129"/>
+      <c r="AW20" s="126"/>
+      <c r="AX20" s="128"/>
+      <c r="AY20" s="129"/>
+      <c r="AZ20" s="126"/>
+      <c r="BA20" s="125"/>
+      <c r="BB20" s="125"/>
+      <c r="BC20" s="126"/>
+      <c r="BD20" s="126"/>
+      <c r="BE20" s="125"/>
+      <c r="BF20" s="126"/>
+      <c r="BG20" s="128"/>
+      <c r="BH20" s="129"/>
+      <c r="BI20" s="126"/>
+      <c r="BJ20" s="126"/>
+      <c r="BK20" s="128"/>
     </row>
     <row r="21" spans="1:63" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
@@ -6117,65 +6071,65 @@
       <c r="E21" s="55"/>
       <c r="F21" s="56"/>
       <c r="G21" s="53"/>
-      <c r="H21" s="144" t="str">
+      <c r="H21" s="141" t="str">
         <f t="shared" ref="H21:H26" ca="1" si="15">IF(AND($C21="Objetivo",H$7&gt;=$E21,H$7&lt;=$E21+$F21-1),2,IF(AND($C21="Hito",H$7&gt;=$E21,H$7&lt;=$E21+$F21-1),1,""))</f>
         <v/>
       </c>
-      <c r="I21" s="145"/>
-      <c r="J21" s="145"/>
-      <c r="K21" s="145"/>
-      <c r="L21" s="145"/>
-      <c r="M21" s="145"/>
-      <c r="N21" s="145"/>
-      <c r="O21" s="145"/>
-      <c r="P21" s="145"/>
-      <c r="Q21" s="145"/>
-      <c r="R21" s="145"/>
-      <c r="S21" s="145"/>
-      <c r="T21" s="145"/>
-      <c r="U21" s="145"/>
-      <c r="V21" s="145"/>
-      <c r="W21" s="145"/>
-      <c r="X21" s="145"/>
-      <c r="Y21" s="145"/>
-      <c r="Z21" s="145"/>
-      <c r="AA21" s="145"/>
-      <c r="AB21" s="145"/>
-      <c r="AC21" s="145"/>
-      <c r="AD21" s="145"/>
-      <c r="AE21" s="145"/>
-      <c r="AF21" s="145"/>
-      <c r="AG21" s="145"/>
-      <c r="AH21" s="145"/>
-      <c r="AI21" s="145"/>
-      <c r="AJ21" s="145"/>
-      <c r="AK21" s="145"/>
-      <c r="AL21" s="145"/>
-      <c r="AM21" s="145"/>
-      <c r="AN21" s="145"/>
-      <c r="AO21" s="145"/>
-      <c r="AP21" s="145"/>
-      <c r="AQ21" s="145"/>
-      <c r="AR21" s="145"/>
-      <c r="AS21" s="145"/>
-      <c r="AT21" s="145"/>
-      <c r="AU21" s="145"/>
-      <c r="AV21" s="145"/>
-      <c r="AW21" s="145"/>
-      <c r="AX21" s="145"/>
-      <c r="AY21" s="145"/>
-      <c r="AZ21" s="145"/>
-      <c r="BA21" s="145"/>
-      <c r="BB21" s="145"/>
-      <c r="BC21" s="145"/>
-      <c r="BD21" s="145"/>
-      <c r="BE21" s="145"/>
-      <c r="BF21" s="145"/>
-      <c r="BG21" s="145"/>
-      <c r="BH21" s="145"/>
-      <c r="BI21" s="145"/>
-      <c r="BJ21" s="145"/>
-      <c r="BK21" s="146"/>
+      <c r="I21" s="142"/>
+      <c r="J21" s="142"/>
+      <c r="K21" s="142"/>
+      <c r="L21" s="142"/>
+      <c r="M21" s="142"/>
+      <c r="N21" s="142"/>
+      <c r="O21" s="142"/>
+      <c r="P21" s="142"/>
+      <c r="Q21" s="142"/>
+      <c r="R21" s="142"/>
+      <c r="S21" s="142"/>
+      <c r="T21" s="142"/>
+      <c r="U21" s="142"/>
+      <c r="V21" s="142"/>
+      <c r="W21" s="142"/>
+      <c r="X21" s="142"/>
+      <c r="Y21" s="142"/>
+      <c r="Z21" s="142"/>
+      <c r="AA21" s="142"/>
+      <c r="AB21" s="142"/>
+      <c r="AC21" s="142"/>
+      <c r="AD21" s="142"/>
+      <c r="AE21" s="142"/>
+      <c r="AF21" s="142"/>
+      <c r="AG21" s="142"/>
+      <c r="AH21" s="142"/>
+      <c r="AI21" s="142"/>
+      <c r="AJ21" s="142"/>
+      <c r="AK21" s="142"/>
+      <c r="AL21" s="142"/>
+      <c r="AM21" s="142"/>
+      <c r="AN21" s="142"/>
+      <c r="AO21" s="142"/>
+      <c r="AP21" s="142"/>
+      <c r="AQ21" s="142"/>
+      <c r="AR21" s="142"/>
+      <c r="AS21" s="142"/>
+      <c r="AT21" s="142"/>
+      <c r="AU21" s="142"/>
+      <c r="AV21" s="142"/>
+      <c r="AW21" s="142"/>
+      <c r="AX21" s="142"/>
+      <c r="AY21" s="142"/>
+      <c r="AZ21" s="142"/>
+      <c r="BA21" s="142"/>
+      <c r="BB21" s="142"/>
+      <c r="BC21" s="142"/>
+      <c r="BD21" s="142"/>
+      <c r="BE21" s="142"/>
+      <c r="BF21" s="142"/>
+      <c r="BG21" s="142"/>
+      <c r="BH21" s="142"/>
+      <c r="BI21" s="142"/>
+      <c r="BJ21" s="142"/>
+      <c r="BK21" s="143"/>
     </row>
     <row r="22" spans="1:63" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
@@ -7634,7 +7588,7 @@
         <v>23</v>
       </c>
       <c r="D30" s="54">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E30" s="55">
         <f t="shared" si="21"/>
@@ -7711,65 +7665,65 @@
       <c r="E31" s="55"/>
       <c r="F31" s="56"/>
       <c r="G31" s="53"/>
-      <c r="H31" s="135" t="str">
-        <f t="shared" ref="H31:Q37" ca="1" si="22">IF(AND($C31="Objetivo",H$7&gt;=$E31,H$7&lt;=$E31+$F31-1),2,IF(AND($C31="Hito",H$7&gt;=$E31,H$7&lt;=$E31+$F31-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="I31" s="136"/>
-      <c r="J31" s="136"/>
-      <c r="K31" s="136"/>
-      <c r="L31" s="136"/>
-      <c r="M31" s="136"/>
-      <c r="N31" s="136"/>
-      <c r="O31" s="136"/>
-      <c r="P31" s="136"/>
-      <c r="Q31" s="136"/>
-      <c r="R31" s="136"/>
-      <c r="S31" s="136"/>
-      <c r="T31" s="136"/>
-      <c r="U31" s="136"/>
-      <c r="V31" s="136"/>
-      <c r="W31" s="136"/>
-      <c r="X31" s="136"/>
-      <c r="Y31" s="136"/>
-      <c r="Z31" s="136"/>
-      <c r="AA31" s="136"/>
-      <c r="AB31" s="136"/>
-      <c r="AC31" s="136"/>
-      <c r="AD31" s="136"/>
-      <c r="AE31" s="136"/>
-      <c r="AF31" s="136"/>
-      <c r="AG31" s="136"/>
-      <c r="AH31" s="136"/>
-      <c r="AI31" s="136"/>
-      <c r="AJ31" s="136"/>
-      <c r="AK31" s="136"/>
-      <c r="AL31" s="136"/>
-      <c r="AM31" s="136"/>
-      <c r="AN31" s="136"/>
-      <c r="AO31" s="136"/>
-      <c r="AP31" s="136"/>
-      <c r="AQ31" s="136"/>
-      <c r="AR31" s="136"/>
-      <c r="AS31" s="136"/>
-      <c r="AT31" s="136"/>
-      <c r="AU31" s="136"/>
-      <c r="AV31" s="136"/>
-      <c r="AW31" s="136"/>
-      <c r="AX31" s="136"/>
-      <c r="AY31" s="136"/>
-      <c r="AZ31" s="136"/>
-      <c r="BA31" s="136"/>
-      <c r="BB31" s="136"/>
-      <c r="BC31" s="136"/>
-      <c r="BD31" s="136"/>
-      <c r="BE31" s="136"/>
-      <c r="BF31" s="136"/>
-      <c r="BG31" s="136"/>
-      <c r="BH31" s="136"/>
-      <c r="BI31" s="136"/>
-      <c r="BJ31" s="136"/>
-      <c r="BK31" s="137"/>
+      <c r="H31" s="132" t="str">
+        <f t="shared" ref="H31:Q34" ca="1" si="22">IF(AND($C31="Objetivo",H$7&gt;=$E31,H$7&lt;=$E31+$F31-1),2,IF(AND($C31="Hito",H$7&gt;=$E31,H$7&lt;=$E31+$F31-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="I31" s="133"/>
+      <c r="J31" s="133"/>
+      <c r="K31" s="133"/>
+      <c r="L31" s="133"/>
+      <c r="M31" s="133"/>
+      <c r="N31" s="133"/>
+      <c r="O31" s="133"/>
+      <c r="P31" s="133"/>
+      <c r="Q31" s="133"/>
+      <c r="R31" s="133"/>
+      <c r="S31" s="133"/>
+      <c r="T31" s="133"/>
+      <c r="U31" s="133"/>
+      <c r="V31" s="133"/>
+      <c r="W31" s="133"/>
+      <c r="X31" s="133"/>
+      <c r="Y31" s="133"/>
+      <c r="Z31" s="133"/>
+      <c r="AA31" s="133"/>
+      <c r="AB31" s="133"/>
+      <c r="AC31" s="133"/>
+      <c r="AD31" s="133"/>
+      <c r="AE31" s="133"/>
+      <c r="AF31" s="133"/>
+      <c r="AG31" s="133"/>
+      <c r="AH31" s="133"/>
+      <c r="AI31" s="133"/>
+      <c r="AJ31" s="133"/>
+      <c r="AK31" s="133"/>
+      <c r="AL31" s="133"/>
+      <c r="AM31" s="133"/>
+      <c r="AN31" s="133"/>
+      <c r="AO31" s="133"/>
+      <c r="AP31" s="133"/>
+      <c r="AQ31" s="133"/>
+      <c r="AR31" s="133"/>
+      <c r="AS31" s="133"/>
+      <c r="AT31" s="133"/>
+      <c r="AU31" s="133"/>
+      <c r="AV31" s="133"/>
+      <c r="AW31" s="133"/>
+      <c r="AX31" s="133"/>
+      <c r="AY31" s="133"/>
+      <c r="AZ31" s="133"/>
+      <c r="BA31" s="133"/>
+      <c r="BB31" s="133"/>
+      <c r="BC31" s="133"/>
+      <c r="BD31" s="133"/>
+      <c r="BE31" s="133"/>
+      <c r="BF31" s="133"/>
+      <c r="BG31" s="133"/>
+      <c r="BH31" s="133"/>
+      <c r="BI31" s="133"/>
+      <c r="BJ31" s="133"/>
+      <c r="BK31" s="134"/>
     </row>
     <row r="32" spans="1:63" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
@@ -7780,7 +7734,7 @@
         <v>23</v>
       </c>
       <c r="D32" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="55">
         <f>E30+F30</f>
@@ -7831,7 +7785,7 @@
         <v/>
       </c>
       <c r="R32" s="24" t="str">
-        <f t="shared" ref="R32:AA37" ca="1" si="23">IF(AND($C32="Objetivo",R$7&gt;=$E32,R$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",R$7&gt;=$E32,R$7&lt;=$E32+$F32-1),1,""))</f>
+        <f t="shared" ref="R32:AA34" ca="1" si="23">IF(AND($C32="Objetivo",R$7&gt;=$E32,R$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",R$7&gt;=$E32,R$7&lt;=$E32+$F32-1),1,""))</f>
         <v/>
       </c>
       <c r="S32" s="24" t="str">
@@ -7871,7 +7825,7 @@
         <v/>
       </c>
       <c r="AB32" s="24" t="str">
-        <f t="shared" ref="AB32:AK37" ca="1" si="24">IF(AND($C32="Objetivo",AB$7&gt;=$E32,AB$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",AB$7&gt;=$E32,AB$7&lt;=$E32+$F32-1),1,""))</f>
+        <f t="shared" ref="AB32:AK34" ca="1" si="24">IF(AND($C32="Objetivo",AB$7&gt;=$E32,AB$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",AB$7&gt;=$E32,AB$7&lt;=$E32+$F32-1),1,""))</f>
         <v/>
       </c>
       <c r="AC32" s="24" t="str">
@@ -7911,7 +7865,7 @@
         <v/>
       </c>
       <c r="AL32" s="24" t="str">
-        <f t="shared" ref="AL32:AU37" ca="1" si="25">IF(AND($C32="Objetivo",AL$7&gt;=$E32,AL$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",AL$7&gt;=$E32,AL$7&lt;=$E32+$F32-1),1,""))</f>
+        <f t="shared" ref="AL32:AU34" ca="1" si="25">IF(AND($C32="Objetivo",AL$7&gt;=$E32,AL$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",AL$7&gt;=$E32,AL$7&lt;=$E32+$F32-1),1,""))</f>
         <v/>
       </c>
       <c r="AM32" s="24" t="str">
@@ -7951,7 +7905,7 @@
         <v/>
       </c>
       <c r="AV32" s="24" t="str">
-        <f t="shared" ref="AV32:BE37" ca="1" si="26">IF(AND($C32="Objetivo",AV$7&gt;=$E32,AV$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",AV$7&gt;=$E32,AV$7&lt;=$E32+$F32-1),1,""))</f>
+        <f t="shared" ref="AV32:BE34" ca="1" si="26">IF(AND($C32="Objetivo",AV$7&gt;=$E32,AV$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",AV$7&gt;=$E32,AV$7&lt;=$E32+$F32-1),1,""))</f>
         <v/>
       </c>
       <c r="AW32" s="24" t="str">
@@ -7991,7 +7945,7 @@
         <v/>
       </c>
       <c r="BF32" s="24" t="str">
-        <f t="shared" ref="BF32:BK37" ca="1" si="27">IF(AND($C32="Objetivo",BF$7&gt;=$E32,BF$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",BF$7&gt;=$E32,BF$7&lt;=$E32+$F32-1),1,""))</f>
+        <f t="shared" ref="BF32:BK34" ca="1" si="27">IF(AND($C32="Objetivo",BF$7&gt;=$E32,BF$7&lt;=$E32+$F32-1),2,IF(AND($C32="Hito",BF$7&gt;=$E32,BF$7&lt;=$E32+$F32-1),1,""))</f>
         <v/>
       </c>
       <c r="BG32" s="24" t="str">
@@ -8015,7 +7969,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:63" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="57" t="s">
         <v>59</v>
@@ -8024,7 +7978,7 @@
         <v>24</v>
       </c>
       <c r="D33" s="54">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E33" s="55">
         <v>45752</v>
@@ -8258,7 +8212,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:63" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="57" t="s">
         <v>60</v>
@@ -8267,7 +8221,7 @@
         <v>24</v>
       </c>
       <c r="D34" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="55">
         <v>45815</v>
@@ -8501,780 +8455,73 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="56"/>
+    <row r="35" spans="1:63" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35" s="2"/>
+      <c r="F35"/>
       <c r="G35" s="53"/>
-      <c r="H35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="I35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="J35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="K35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="L35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="M35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="N35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="O35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="P35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="Q35" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="R35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="S35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="T35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="U35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="V35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="W35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="X35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="Y35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="Z35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AA35" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AB35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AH35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AI35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AJ35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AK35" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AL35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AM35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AN35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AO35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AP35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AQ35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AR35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AS35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AT35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AU35" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AV35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AW35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AX35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AY35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AZ35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BA35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BB35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BC35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BD35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BE35" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BF35" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BG35" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BH35" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BI35" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BJ35" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BK35" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="79"/>
+      <c r="P35" s="79"/>
+      <c r="Q35" s="79"/>
+      <c r="R35" s="79"/>
+      <c r="S35" s="79"/>
+      <c r="T35" s="79"/>
+      <c r="U35" s="79"/>
+      <c r="V35" s="79"/>
+      <c r="W35" s="79"/>
+      <c r="X35" s="79"/>
+      <c r="Y35" s="79"/>
+      <c r="Z35" s="79"/>
+      <c r="AA35" s="79"/>
+      <c r="AB35" s="79"/>
+      <c r="AC35" s="79"/>
+      <c r="AD35" s="79"/>
+      <c r="AE35" s="79"/>
+      <c r="AF35" s="79"/>
+      <c r="AG35" s="79"/>
+      <c r="AH35" s="79"/>
+      <c r="AI35" s="79"/>
+      <c r="AJ35" s="79"/>
+      <c r="AK35" s="79"/>
+      <c r="AL35" s="79"/>
+      <c r="AM35" s="79"/>
+      <c r="AN35" s="79"/>
+      <c r="AO35" s="79"/>
+      <c r="AP35" s="79"/>
+      <c r="AQ35" s="79"/>
+      <c r="AR35" s="79"/>
+      <c r="AS35" s="79"/>
+      <c r="AT35" s="79"/>
+      <c r="AU35" s="79"/>
+      <c r="AV35" s="79"/>
+      <c r="AW35" s="79"/>
+      <c r="AX35" s="79"/>
+      <c r="AY35" s="79"/>
+      <c r="AZ35" s="79"/>
+      <c r="BA35" s="79"/>
+      <c r="BB35" s="79"/>
+      <c r="BC35" s="79"/>
+      <c r="BD35" s="79"/>
+      <c r="BE35" s="79"/>
+      <c r="BF35" s="79"/>
+      <c r="BG35" s="79"/>
+      <c r="BH35" s="79"/>
+      <c r="BI35" s="79"/>
+      <c r="BJ35" s="79"/>
+      <c r="BK35" s="79"/>
     </row>
-    <row r="36" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="I36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="J36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="K36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="L36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="M36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="N36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="O36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="P36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="Q36" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="R36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="S36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="T36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="U36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="V36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="W36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="X36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="Y36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="Z36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AA36" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AB36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AH36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AI36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AJ36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AK36" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AL36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AM36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AN36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AO36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AP36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AQ36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AR36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AS36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AT36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AU36" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AV36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AW36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AX36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AY36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AZ36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BA36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BB36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BC36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BD36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BE36" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BF36" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BG36" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BH36" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BI36" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BJ36" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BK36" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="I37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="J37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="K37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="L37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="M37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="N37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="O37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="P37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="Q37" s="24" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="R37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="S37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="T37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="U37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="V37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="W37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="X37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="Y37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="Z37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AA37" s="24" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AB37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AH37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AI37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AJ37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AK37" s="24" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AL37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AM37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AN37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AO37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AP37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AQ37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AR37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AS37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AT37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AU37" s="24" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AV37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AW37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AX37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AY37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="AZ37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BA37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BB37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BC37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BD37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BE37" s="24" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BF37" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BG37" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BH37" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BI37" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BJ37" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BK37" s="24" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v/>
-      </c>
-      <c r="BL37" s="81"/>
-    </row>
-    <row r="38" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="101" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="79"/>
-      <c r="I38" s="79"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="79"/>
-      <c r="N38" s="79"/>
-      <c r="O38" s="79"/>
-      <c r="P38" s="79"/>
-      <c r="Q38" s="79"/>
-      <c r="R38" s="79"/>
-      <c r="S38" s="79"/>
-      <c r="T38" s="79"/>
-      <c r="U38" s="79"/>
-      <c r="V38" s="79"/>
-      <c r="W38" s="79"/>
-      <c r="X38" s="79"/>
-      <c r="Y38" s="79"/>
-      <c r="Z38" s="79"/>
-      <c r="AA38" s="79"/>
-      <c r="AB38" s="79"/>
-      <c r="AC38" s="79"/>
-      <c r="AD38" s="79"/>
-      <c r="AE38" s="79"/>
-      <c r="AF38" s="79"/>
-      <c r="AG38" s="79"/>
-      <c r="AH38" s="79"/>
-      <c r="AI38" s="79"/>
-      <c r="AJ38" s="79"/>
-      <c r="AK38" s="79"/>
-      <c r="AL38" s="79"/>
-      <c r="AM38" s="79"/>
-      <c r="AN38" s="79"/>
-      <c r="AO38" s="79"/>
-      <c r="AP38" s="79"/>
-      <c r="AQ38" s="79"/>
-      <c r="AR38" s="79"/>
-      <c r="AS38" s="79"/>
-      <c r="AT38" s="79"/>
-      <c r="AU38" s="79"/>
-      <c r="AV38" s="79"/>
-      <c r="AW38" s="79"/>
-      <c r="AX38" s="79"/>
-      <c r="AY38" s="79"/>
-      <c r="AZ38" s="79"/>
-      <c r="BA38" s="79"/>
-      <c r="BB38" s="79"/>
-      <c r="BC38" s="79"/>
-      <c r="BD38" s="79"/>
-      <c r="BE38" s="79"/>
-      <c r="BF38" s="79"/>
-      <c r="BG38" s="79"/>
-      <c r="BH38" s="79"/>
-      <c r="BI38" s="79"/>
-      <c r="BJ38" s="79"/>
-      <c r="BK38" s="79"/>
-    </row>
-    <row r="39" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F39" s="11"/>
-      <c r="G39" s="3"/>
+    <row r="36" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G36" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -9291,7 +8538,7 @@
     <mergeCell ref="W4:Z4"/>
     <mergeCell ref="AB4:AE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D9:D38">
+  <conditionalFormatting sqref="D9:D34">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9315,38 +8562,38 @@
       <formula>AND(H$7&lt;=EOMONTH($H$7,1),H$7&gt;EOMONTH($H$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BK10 H11 H12:BK14 H15 H16:BK20 H21 H22:BK30 H31 H32:BK38">
-    <cfRule type="expression" dxfId="24" priority="1">
+  <conditionalFormatting sqref="H7:BK10 H11 H12:BK14 H15 H21 H22:BK30 H31 H32:BK35 H16:BK20">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>AND(TODAY()&gt;=H$7,TODAY()&lt;I$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10:BK10 H11 H12:BK14 H15 H16:BK20 H21 H22:BK30 H31 H32:BK37">
-    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
+  <conditionalFormatting sqref="H10:BK10 H11 H12:BK14 H15 H21 H22:BK30 H31 H32:BK34 H16:BK20">
+    <cfRule type="expression" dxfId="4" priority="34" stopIfTrue="1">
       <formula>AND($C10="Riesgo bajo",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="35" stopIfTrue="1">
       <formula>AND($C10="Riesgo alto",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="36" stopIfTrue="1">
       <formula>AND($C10="Según lo previsto",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="37" stopIfTrue="1">
       <formula>AND($C10="Riesgo medio",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="38" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BK6">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>AND(I$7&lt;=EOMONTH($H$7,2),I$7&gt;EOMONTH($H$7,0),I$7&gt;EOMONTH($H$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="13">
+  <dataValidations count="12">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Incremento de desplazamiento" prompt="Al cambiar este número, se desplazará la vista del diagrama de Gantt." sqref="C7" xr:uid="{662A47A0-7258-440E-8D71-BC54CBC9C651}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C37" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C34" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
       <formula1>"Objetivo,Hito,Según lo previsto, Riesgo bajo, Riesgo medio, Riesgo alto"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{218D9212-09C8-4DA2-9014-64503951B170}">
@@ -9360,8 +8607,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hay una barra de desplazamiento entre las celdas I8 y BL8. _x000a_Para avanzar o retroceder en la escala de tiempo, escriba un valor de 0 o superior en la celda C7._x000a_El valor 0 le lleva al principio del gráfico." sqref="A8" xr:uid="{737D7247-B514-41B2-94CC-2F538E17DE66}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="La fila tiene encabezados de la programación del proyecto. Hay información de la programación entre B9 y G9. Las celdas I9 a BL9 tienen la primera letra de los días de la fecha anterior al encabezado._x000a_Los gráficos de escala de tiempo se autogeneran." sqref="A9" xr:uid="{6AB925DC-9BC9-4EC3-A848-25121289EECD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba información del proyecto desde la celda B11 hasta la G11. _x000a_Escriba la descripción del hito, seleccione una categoría, asigne a alguien a la tarea y escriba el progreso, fecha de inicio y días para que la tarea empiece el gráfico._x000a_" sqref="A11" xr:uid="{77315CCB-C571-42B0-8983-9C17BB04F75F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta fila marca el final de los datos del hito de Gantt. NO escriba nada en esta fila. _x000a_Para agregar más elementos, inserte las nuevas filas encima de esta._x000a_" sqref="A38" xr:uid="{659FD5CB-B62B-4854-B8A9-29F1F70930AC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta es una fila vacía" sqref="A37" xr:uid="{60F6BB2A-523D-41BA-B324-85E19FB9FF7E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta fila marca el final de los datos del hito de Gantt. NO escriba nada en esta fila. _x000a_Para agregar más elementos, inserte las nuevas filas encima de esta._x000a_" sqref="A35" xr:uid="{659FD5CB-B62B-4854-B8A9-29F1F70930AC}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -9388,26 +8634,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D9:D38</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="33" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>H10:BK10 H22:BK30 H21 H16:BK20 H15 H12:BK14 H11 H32:BK37 H31</xm:sqref>
+          <xm:sqref>D9:D34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{A1EFF969-3CBB-4DB2-A4C9-47B01FE32C86}">
@@ -9426,7 +8653,26 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H38:BK38</xm:sqref>
+          <xm:sqref>H35:BK35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="53" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H10:BK10 H22:BK30 H21 H15 H12:BK14 H11 H32:BK34 H31 H16:BK20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -9441,7 +8687,7 @@
   </sheetPr>
   <dimension ref="A1:BP38"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9459,27 +8705,27 @@
     <row r="1" spans="1:68" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:68" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="150"/>
-      <c r="L2" s="150"/>
-      <c r="M2" s="150"/>
-      <c r="N2" s="150"/>
-      <c r="O2" s="151"/>
-      <c r="P2" s="152"/>
-      <c r="Q2" s="152"/>
-      <c r="R2" s="152"/>
-      <c r="S2" s="152"/>
-      <c r="T2" s="152"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="147"/>
+      <c r="O2" s="148"/>
+      <c r="P2" s="149"/>
+      <c r="Q2" s="149"/>
+      <c r="R2" s="149"/>
+      <c r="S2" s="149"/>
+      <c r="T2" s="149"/>
       <c r="U2" s="18"/>
       <c r="V2" s="18"/>
       <c r="W2" s="18"/>
@@ -9606,40 +8852,40 @@
         <v>30</v>
       </c>
       <c r="H4" s="27"/>
-      <c r="I4" s="141" t="s">
+      <c r="I4" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="138"/>
       <c r="M4" s="30"/>
-      <c r="N4" s="142" t="s">
+      <c r="N4" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="142"/>
-      <c r="P4" s="142"/>
-      <c r="Q4" s="142"/>
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="139"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="143" t="s">
+      <c r="S4" s="140" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="143"/>
-      <c r="U4" s="143"/>
-      <c r="V4" s="143"/>
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
+      <c r="V4" s="140"/>
       <c r="W4" s="30"/>
-      <c r="X4" s="147" t="s">
+      <c r="X4" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" s="147"/>
-      <c r="Z4" s="147"/>
-      <c r="AA4" s="147"/>
+      <c r="Y4" s="144"/>
+      <c r="Z4" s="144"/>
+      <c r="AA4" s="144"/>
       <c r="AB4" s="30"/>
-      <c r="AC4" s="148" t="s">
+      <c r="AC4" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="AD4" s="148"/>
-      <c r="AE4" s="148"/>
-      <c r="AF4" s="148"/>
+      <c r="AD4" s="145"/>
+      <c r="AE4" s="145"/>
+      <c r="AF4" s="145"/>
       <c r="AG4" s="30"/>
       <c r="AH4" s="30"/>
       <c r="AI4" s="30"/>
@@ -9750,7 +8996,7 @@
       </c>
       <c r="C6" s="32" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Hitos435[Inicio])=0,TODAY(),B11(Hitos435[Inicio])),TODAY())</f>
-        <v>45804</v>
+        <v>45823</v>
       </c>
       <c r="D6" s="115"/>
       <c r="E6" s="30"/>
@@ -9759,7 +9005,7 @@
       <c r="H6" s="27"/>
       <c r="I6" s="86" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>mayo</v>
+        <v>junio</v>
       </c>
       <c r="J6" s="86"/>
       <c r="K6" s="86"/>
@@ -9769,7 +9015,7 @@
       <c r="O6" s="86"/>
       <c r="P6" s="86" t="str">
         <f ca="1">IF(TEXT(P7,"mmmm")=I6,"",TEXT(P7,"mmmm"))</f>
-        <v>junio</v>
+        <v/>
       </c>
       <c r="Q6" s="86"/>
       <c r="R6" s="86"/>
@@ -9789,7 +9035,7 @@
       <c r="AC6" s="86"/>
       <c r="AD6" s="86" t="str">
         <f ca="1">IF(OR(TEXT(AD7,"mmmm")=W6,TEXT(AD7,"mmmm")=P6,TEXT(AD7,"mmmm")=I6),"",TEXT(AD7,"mmmm"))</f>
-        <v/>
+        <v>julio</v>
       </c>
       <c r="AE6" s="86"/>
       <c r="AF6" s="86"/>
@@ -9809,7 +9055,7 @@
       <c r="AQ6" s="86"/>
       <c r="AR6" s="86" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v>julio</v>
+        <v/>
       </c>
       <c r="AS6" s="86"/>
       <c r="AT6" s="86"/>
@@ -9829,7 +9075,7 @@
       <c r="BE6" s="58"/>
       <c r="BF6" s="58" t="str">
         <f ca="1">IF(OR(TEXT(BF7,"mmmm")=AY6,TEXT(BF7,"mmmm")=AR6,TEXT(BF7,"mmmm")=AK6,TEXT(BF7,"mmmm")=AD6),"",TEXT(BF7,"mmmm"))</f>
-        <v/>
+        <v>agosto</v>
       </c>
       <c r="BG6" s="58"/>
       <c r="BH6" s="58"/>
@@ -9854,227 +9100,227 @@
       <c r="H7" s="27"/>
       <c r="I7" s="116">
         <f ca="1">IFERROR(Inicio_del_proyecto+Incremento_de_desplazamiento,TODAY())</f>
-        <v>45805</v>
+        <v>45824</v>
       </c>
       <c r="J7" s="117">
         <f ca="1">I7+1</f>
-        <v>45806</v>
+        <v>45825</v>
       </c>
       <c r="K7" s="117">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45807</v>
+        <v>45826</v>
       </c>
       <c r="L7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45808</v>
+        <v>45827</v>
       </c>
       <c r="M7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45809</v>
+        <v>45828</v>
       </c>
       <c r="N7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45810</v>
+        <v>45829</v>
       </c>
       <c r="O7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>45811</v>
+        <v>45830</v>
       </c>
       <c r="P7" s="117">
         <f ca="1">O7+1</f>
-        <v>45812</v>
+        <v>45831</v>
       </c>
       <c r="Q7" s="117">
         <f ca="1">P7+1</f>
-        <v>45813</v>
+        <v>45832</v>
       </c>
       <c r="R7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45814</v>
+        <v>45833</v>
       </c>
       <c r="S7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45815</v>
+        <v>45834</v>
       </c>
       <c r="T7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45816</v>
+        <v>45835</v>
       </c>
       <c r="U7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45817</v>
+        <v>45836</v>
       </c>
       <c r="V7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>45818</v>
+        <v>45837</v>
       </c>
       <c r="W7" s="117">
         <f ca="1">V7+1</f>
-        <v>45819</v>
+        <v>45838</v>
       </c>
       <c r="X7" s="117">
         <f ca="1">W7+1</f>
-        <v>45820</v>
+        <v>45839</v>
       </c>
       <c r="Y7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45821</v>
+        <v>45840</v>
       </c>
       <c r="Z7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45822</v>
+        <v>45841</v>
       </c>
       <c r="AA7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45823</v>
+        <v>45842</v>
       </c>
       <c r="AB7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45824</v>
+        <v>45843</v>
       </c>
       <c r="AC7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>45825</v>
+        <v>45844</v>
       </c>
       <c r="AD7" s="117">
         <f ca="1">AC7+1</f>
-        <v>45826</v>
+        <v>45845</v>
       </c>
       <c r="AE7" s="117">
         <f ca="1">AD7+1</f>
-        <v>45827</v>
+        <v>45846</v>
       </c>
       <c r="AF7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45828</v>
+        <v>45847</v>
       </c>
       <c r="AG7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45829</v>
+        <v>45848</v>
       </c>
       <c r="AH7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45830</v>
+        <v>45849</v>
       </c>
       <c r="AI7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45831</v>
+        <v>45850</v>
       </c>
       <c r="AJ7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>45832</v>
+        <v>45851</v>
       </c>
       <c r="AK7" s="117">
         <f ca="1">AJ7+1</f>
-        <v>45833</v>
+        <v>45852</v>
       </c>
       <c r="AL7" s="117">
         <f ca="1">AK7+1</f>
-        <v>45834</v>
+        <v>45853</v>
       </c>
       <c r="AM7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45835</v>
+        <v>45854</v>
       </c>
       <c r="AN7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45836</v>
+        <v>45855</v>
       </c>
       <c r="AO7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45837</v>
+        <v>45856</v>
       </c>
       <c r="AP7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45838</v>
+        <v>45857</v>
       </c>
       <c r="AQ7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>45839</v>
+        <v>45858</v>
       </c>
       <c r="AR7" s="117">
         <f ca="1">AQ7+1</f>
-        <v>45840</v>
+        <v>45859</v>
       </c>
       <c r="AS7" s="117">
         <f ca="1">AR7+1</f>
-        <v>45841</v>
+        <v>45860</v>
       </c>
       <c r="AT7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45842</v>
+        <v>45861</v>
       </c>
       <c r="AU7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45843</v>
+        <v>45862</v>
       </c>
       <c r="AV7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45844</v>
+        <v>45863</v>
       </c>
       <c r="AW7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>45845</v>
+        <v>45864</v>
       </c>
       <c r="AX7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>45846</v>
+        <v>45865</v>
       </c>
       <c r="AY7" s="117">
         <f ca="1">AX7+1</f>
-        <v>45847</v>
+        <v>45866</v>
       </c>
       <c r="AZ7" s="117">
         <f ca="1">AY7+1</f>
-        <v>45848</v>
+        <v>45867</v>
       </c>
       <c r="BA7" s="117">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>45849</v>
+        <v>45868</v>
       </c>
       <c r="BB7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>45850</v>
+        <v>45869</v>
       </c>
       <c r="BC7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>45851</v>
+        <v>45870</v>
       </c>
       <c r="BD7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>45852</v>
+        <v>45871</v>
       </c>
       <c r="BE7" s="118">
         <f t="shared" ca="1" si="1"/>
-        <v>45853</v>
+        <v>45872</v>
       </c>
       <c r="BF7" s="117">
         <f ca="1">BE7+1</f>
-        <v>45854</v>
+        <v>45873</v>
       </c>
       <c r="BG7" s="117">
         <f ca="1">BF7+1</f>
-        <v>45855</v>
+        <v>45874</v>
       </c>
       <c r="BH7" s="117">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>45856</v>
+        <v>45875</v>
       </c>
       <c r="BI7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>45857</v>
+        <v>45876</v>
       </c>
       <c r="BJ7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>45858</v>
+        <v>45877</v>
       </c>
       <c r="BK7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>45859</v>
+        <v>45878</v>
       </c>
       <c r="BL7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>45860</v>
+        <v>45879</v>
       </c>
       <c r="BM7" s="30"/>
     </row>
@@ -10168,227 +9414,227 @@
       <c r="H9" s="43"/>
       <c r="I9" s="35" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="J9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="K9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="L9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="M9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="N9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="O9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="P9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="Q9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="R9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="S9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="T9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="U9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="V9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="W9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="X9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="Y9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="Z9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="AA9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="AB9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="AC9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AD9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="AE9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="AF9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AG9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="AH9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="AI9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="AJ9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AK9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="AL9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="AM9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AN9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="AO9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="AP9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="AQ9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AR9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="AS9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="AT9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AU9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="AV9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="AW9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="AX9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AY9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="AZ9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="BA9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="BB9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="BC9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="BD9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="BE9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="BF9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="BG9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="BH9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="BI9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="BJ9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="BK9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="BL9" s="35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="BM9" s="30"/>
     </row>
@@ -10712,7 +9958,7 @@
       </c>
       <c r="F12" s="21">
         <f ca="1">TODAY()</f>
-        <v>45804</v>
+        <v>45823</v>
       </c>
       <c r="G12" s="22">
         <v>3</v>
@@ -10956,7 +10202,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="21">
         <f ca="1">TODAY()+5</f>
-        <v>45809</v>
+        <v>45828</v>
       </c>
       <c r="G13" s="22">
         <v>1</v>
@@ -11202,7 +10448,7 @@
       </c>
       <c r="F14" s="21">
         <f ca="1">F12-3</f>
-        <v>45801</v>
+        <v>45820</v>
       </c>
       <c r="G14" s="22">
         <v>10</v>
@@ -11446,7 +10692,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="21">
         <f ca="1">F12+20</f>
-        <v>45824</v>
+        <v>45843</v>
       </c>
       <c r="G15" s="22">
         <v>1</v>
@@ -11692,7 +10938,7 @@
       </c>
       <c r="F16" s="21">
         <f ca="1">F12+6</f>
-        <v>45810</v>
+        <v>45829</v>
       </c>
       <c r="G16" s="22">
         <v>6</v>
@@ -12175,7 +11421,7 @@
       </c>
       <c r="F18" s="21">
         <f ca="1">F12+6</f>
-        <v>45810</v>
+        <v>45829</v>
       </c>
       <c r="G18" s="22">
         <v>13</v>
@@ -12421,7 +11667,7 @@
       </c>
       <c r="F19" s="21">
         <f ca="1">F18+2</f>
-        <v>45812</v>
+        <v>45831</v>
       </c>
       <c r="G19" s="22">
         <v>9</v>
@@ -12667,7 +11913,7 @@
       </c>
       <c r="F20" s="21">
         <f ca="1">F19+5</f>
-        <v>45817</v>
+        <v>45836</v>
       </c>
       <c r="G20" s="22">
         <v>11</v>
@@ -12911,7 +12157,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="21">
         <f ca="1">F20+2</f>
-        <v>45819</v>
+        <v>45838</v>
       </c>
       <c r="G21" s="22">
         <v>1</v>
@@ -13153,7 +12399,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="21">
         <f ca="1">F21+1</f>
-        <v>45820</v>
+        <v>45839</v>
       </c>
       <c r="G22" s="22">
         <v>24</v>
@@ -13634,7 +12880,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="21">
         <f ca="1">F12+15</f>
-        <v>45819</v>
+        <v>45838</v>
       </c>
       <c r="G24" s="22">
         <v>4</v>
@@ -13878,7 +13124,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="21">
         <f ca="1">F24+3</f>
-        <v>45822</v>
+        <v>45841</v>
       </c>
       <c r="G25" s="22">
         <v>14</v>
@@ -14122,7 +13368,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="21">
         <f ca="1">F25+15</f>
-        <v>45837</v>
+        <v>45856</v>
       </c>
       <c r="G26" s="22">
         <v>6</v>
@@ -14366,7 +13612,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="21">
         <f ca="1">F21+22</f>
-        <v>45841</v>
+        <v>45860</v>
       </c>
       <c r="G27" s="22">
         <v>3</v>
@@ -14610,7 +13856,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="21">
         <f ca="1">F16</f>
-        <v>45810</v>
+        <v>45829</v>
       </c>
       <c r="G28" s="22">
         <v>19</v>
@@ -15089,7 +14335,7 @@
       <c r="E30" s="20"/>
       <c r="F30" s="21">
         <f ca="1">F27+3</f>
-        <v>45844</v>
+        <v>45863</v>
       </c>
       <c r="G30" s="22">
         <v>15</v>
@@ -15331,7 +14577,7 @@
       <c r="E31" s="20"/>
       <c r="F31" s="21">
         <f ca="1">F30+14</f>
-        <v>45858</v>
+        <v>45877</v>
       </c>
       <c r="G31" s="22">
         <v>5</v>
@@ -15575,7 +14821,7 @@
       <c r="E32" s="20"/>
       <c r="F32" s="21">
         <f ca="1">F31+42</f>
-        <v>45900</v>
+        <v>45919</v>
       </c>
       <c r="G32" s="22">
         <v>1</v>
@@ -16619,39 +15865,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="7" stopIfTrue="1">
       <formula>AND($C10="Riesgo bajo",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="8" stopIfTrue="1">
       <formula>AND($C10="Riesgo alto",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="9" stopIfTrue="1">
       <formula>AND($C10="Según lo previsto",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="10" stopIfTrue="1">
       <formula>AND($C10="Riesgo medio",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16775,27 +16021,27 @@
     <row r="1" spans="1:68" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:68" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="155"/>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="155"/>
-      <c r="S2" s="155"/>
-      <c r="T2" s="155"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="151"/>
+      <c r="J2" s="151"/>
+      <c r="K2" s="151"/>
+      <c r="L2" s="151"/>
+      <c r="M2" s="151"/>
+      <c r="N2" s="151"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
+      <c r="Q2" s="152"/>
+      <c r="R2" s="152"/>
+      <c r="S2" s="152"/>
+      <c r="T2" s="152"/>
       <c r="U2" s="88"/>
       <c r="V2" s="88"/>
       <c r="W2" s="88"/>
@@ -16869,36 +16115,36 @@
         <v>30</v>
       </c>
       <c r="H4" s="68"/>
-      <c r="I4" s="141" t="s">
+      <c r="I4" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="N4" s="142" t="s">
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="138"/>
+      <c r="N4" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="142"/>
-      <c r="P4" s="142"/>
-      <c r="Q4" s="142"/>
-      <c r="S4" s="143" t="s">
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="139"/>
+      <c r="S4" s="140" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="143"/>
-      <c r="U4" s="143"/>
-      <c r="V4" s="143"/>
-      <c r="X4" s="147" t="s">
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
+      <c r="V4" s="140"/>
+      <c r="X4" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" s="147"/>
-      <c r="Z4" s="147"/>
-      <c r="AA4" s="147"/>
-      <c r="AC4" s="148" t="s">
+      <c r="Y4" s="144"/>
+      <c r="Z4" s="144"/>
+      <c r="AA4" s="144"/>
+      <c r="AC4" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="AD4" s="148"/>
-      <c r="AE4" s="148"/>
-      <c r="AF4" s="148"/>
+      <c r="AD4" s="145"/>
+      <c r="AE4" s="145"/>
+      <c r="AF4" s="145"/>
     </row>
     <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
@@ -16919,7 +16165,7 @@
       </c>
       <c r="C6" s="73" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Hitos43524[Inicio])=0,TODAY(),B11(Hitos43524[Inicio])),TODAY())</f>
-        <v>45804</v>
+        <v>45823</v>
       </c>
       <c r="D6" s="73"/>
       <c r="E6" s="68"/>
@@ -16928,7 +16174,7 @@
       <c r="H6" s="68"/>
       <c r="I6" s="83" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>mayo</v>
+        <v>junio</v>
       </c>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
@@ -16938,7 +16184,7 @@
       <c r="O6" s="83"/>
       <c r="P6" s="83" t="str">
         <f ca="1">IF(TEXT(P7,"mmmm")=I6,"",TEXT(P7,"mmmm"))</f>
-        <v>junio</v>
+        <v/>
       </c>
       <c r="Q6" s="83"/>
       <c r="R6" s="83"/>
@@ -16958,7 +16204,7 @@
       <c r="AC6" s="83"/>
       <c r="AD6" s="83" t="str">
         <f ca="1">IF(OR(TEXT(AD7,"mmmm")=W6,TEXT(AD7,"mmmm")=P6,TEXT(AD7,"mmmm")=I6),"",TEXT(AD7,"mmmm"))</f>
-        <v/>
+        <v>julio</v>
       </c>
       <c r="AE6" s="83"/>
       <c r="AF6" s="83"/>
@@ -16978,7 +16224,7 @@
       <c r="AQ6" s="83"/>
       <c r="AR6" s="83" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v>julio</v>
+        <v/>
       </c>
       <c r="AS6" s="83"/>
       <c r="AT6" s="83"/>
@@ -16998,7 +16244,7 @@
       <c r="BE6" s="82"/>
       <c r="BF6" s="82" t="str">
         <f ca="1">IF(OR(TEXT(BF7,"mmmm")=AY6,TEXT(BF7,"mmmm")=AR6,TEXT(BF7,"mmmm")=AK6,TEXT(BF7,"mmmm")=AD6),"",TEXT(BF7,"mmmm"))</f>
-        <v/>
+        <v>agosto</v>
       </c>
       <c r="BG6" s="82"/>
       <c r="BH6" s="82"/>
@@ -17022,227 +16268,227 @@
       <c r="H7" s="75"/>
       <c r="I7" s="107">
         <f ca="1">IFERROR(Inicio_del_proyecto+Incremento_de_desplazamiento,TODAY())</f>
-        <v>45805</v>
+        <v>45824</v>
       </c>
       <c r="J7" s="108">
         <f ca="1">I7+1</f>
-        <v>45806</v>
+        <v>45825</v>
       </c>
       <c r="K7" s="108">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45807</v>
+        <v>45826</v>
       </c>
       <c r="L7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45808</v>
+        <v>45827</v>
       </c>
       <c r="M7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45809</v>
+        <v>45828</v>
       </c>
       <c r="N7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45810</v>
+        <v>45829</v>
       </c>
       <c r="O7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45811</v>
+        <v>45830</v>
       </c>
       <c r="P7" s="108">
         <f ca="1">O7+1</f>
-        <v>45812</v>
+        <v>45831</v>
       </c>
       <c r="Q7" s="108">
         <f ca="1">P7+1</f>
-        <v>45813</v>
+        <v>45832</v>
       </c>
       <c r="R7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45814</v>
+        <v>45833</v>
       </c>
       <c r="S7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45815</v>
+        <v>45834</v>
       </c>
       <c r="T7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45816</v>
+        <v>45835</v>
       </c>
       <c r="U7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45817</v>
+        <v>45836</v>
       </c>
       <c r="V7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45818</v>
+        <v>45837</v>
       </c>
       <c r="W7" s="108">
         <f ca="1">V7+1</f>
-        <v>45819</v>
+        <v>45838</v>
       </c>
       <c r="X7" s="108">
         <f ca="1">W7+1</f>
-        <v>45820</v>
+        <v>45839</v>
       </c>
       <c r="Y7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45821</v>
+        <v>45840</v>
       </c>
       <c r="Z7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45822</v>
+        <v>45841</v>
       </c>
       <c r="AA7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45823</v>
+        <v>45842</v>
       </c>
       <c r="AB7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45824</v>
+        <v>45843</v>
       </c>
       <c r="AC7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45825</v>
+        <v>45844</v>
       </c>
       <c r="AD7" s="108">
         <f ca="1">AC7+1</f>
-        <v>45826</v>
+        <v>45845</v>
       </c>
       <c r="AE7" s="108">
         <f ca="1">AD7+1</f>
-        <v>45827</v>
+        <v>45846</v>
       </c>
       <c r="AF7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45828</v>
+        <v>45847</v>
       </c>
       <c r="AG7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45829</v>
+        <v>45848</v>
       </c>
       <c r="AH7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45830</v>
+        <v>45849</v>
       </c>
       <c r="AI7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45831</v>
+        <v>45850</v>
       </c>
       <c r="AJ7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45832</v>
+        <v>45851</v>
       </c>
       <c r="AK7" s="108">
         <f ca="1">AJ7+1</f>
-        <v>45833</v>
+        <v>45852</v>
       </c>
       <c r="AL7" s="108">
         <f ca="1">AK7+1</f>
-        <v>45834</v>
+        <v>45853</v>
       </c>
       <c r="AM7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45835</v>
+        <v>45854</v>
       </c>
       <c r="AN7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45836</v>
+        <v>45855</v>
       </c>
       <c r="AO7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45837</v>
+        <v>45856</v>
       </c>
       <c r="AP7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45838</v>
+        <v>45857</v>
       </c>
       <c r="AQ7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45839</v>
+        <v>45858</v>
       </c>
       <c r="AR7" s="108">
         <f ca="1">AQ7+1</f>
-        <v>45840</v>
+        <v>45859</v>
       </c>
       <c r="AS7" s="108">
         <f ca="1">AR7+1</f>
-        <v>45841</v>
+        <v>45860</v>
       </c>
       <c r="AT7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45842</v>
+        <v>45861</v>
       </c>
       <c r="AU7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45843</v>
+        <v>45862</v>
       </c>
       <c r="AV7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45844</v>
+        <v>45863</v>
       </c>
       <c r="AW7" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>45845</v>
+        <v>45864</v>
       </c>
       <c r="AX7" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>45846</v>
+        <v>45865</v>
       </c>
       <c r="AY7" s="108">
         <f ca="1">AX7+1</f>
-        <v>45847</v>
+        <v>45866</v>
       </c>
       <c r="AZ7" s="108">
         <f ca="1">AY7+1</f>
-        <v>45848</v>
+        <v>45867</v>
       </c>
       <c r="BA7" s="108">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>45849</v>
+        <v>45868</v>
       </c>
       <c r="BB7" s="108">
         <f t="shared" ca="1" si="1"/>
-        <v>45850</v>
+        <v>45869</v>
       </c>
       <c r="BC7" s="108">
         <f t="shared" ca="1" si="1"/>
-        <v>45851</v>
+        <v>45870</v>
       </c>
       <c r="BD7" s="108">
         <f t="shared" ca="1" si="1"/>
-        <v>45852</v>
+        <v>45871</v>
       </c>
       <c r="BE7" s="109">
         <f t="shared" ca="1" si="1"/>
-        <v>45853</v>
+        <v>45872</v>
       </c>
       <c r="BF7" s="108">
         <f ca="1">BE7+1</f>
-        <v>45854</v>
+        <v>45873</v>
       </c>
       <c r="BG7" s="108">
         <f ca="1">BF7+1</f>
-        <v>45855</v>
+        <v>45874</v>
       </c>
       <c r="BH7" s="108">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>45856</v>
+        <v>45875</v>
       </c>
       <c r="BI7" s="108">
         <f t="shared" ca="1" si="2"/>
-        <v>45857</v>
+        <v>45876</v>
       </c>
       <c r="BJ7" s="108">
         <f t="shared" ca="1" si="2"/>
-        <v>45858</v>
+        <v>45877</v>
       </c>
       <c r="BK7" s="108">
         <f t="shared" ca="1" si="2"/>
-        <v>45859</v>
+        <v>45878</v>
       </c>
       <c r="BL7" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>45860</v>
+        <v>45879</v>
       </c>
     </row>
     <row r="8" spans="1:68" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17334,227 +16580,227 @@
       <c r="H9" s="80"/>
       <c r="I9" s="89" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="J9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="K9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="L9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="M9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="N9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="O9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="P9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="Q9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="R9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="S9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="T9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="U9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="V9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="W9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="X9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="Y9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="Z9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="AA9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="AB9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="AC9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AD9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="AE9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="AF9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AG9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="AH9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="AI9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="AJ9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AK9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="AL9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="AM9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AN9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="AO9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="AP9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="AQ9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AR9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="AS9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="AT9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AU9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="AV9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="AW9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="AX9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AY9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="AZ9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="BA9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="BB9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="BC9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="BD9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="BE9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="BF9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>l</v>
       </c>
       <c r="BG9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>m</v>
       </c>
       <c r="BH9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="BI9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>j</v>
       </c>
       <c r="BJ9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>v</v>
       </c>
       <c r="BK9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>s</v>
       </c>
       <c r="BL9" s="89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
     </row>
     <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -17874,7 +17120,7 @@
       </c>
       <c r="F12" s="55">
         <f ca="1">TODAY()</f>
-        <v>45804</v>
+        <v>45823</v>
       </c>
       <c r="G12" s="56">
         <v>3</v>
@@ -18117,7 +17363,7 @@
       <c r="E13" s="54"/>
       <c r="F13" s="55">
         <f ca="1">TODAY()+5</f>
-        <v>45809</v>
+        <v>45828</v>
       </c>
       <c r="G13" s="56">
         <v>1</v>
@@ -18362,7 +17608,7 @@
       </c>
       <c r="F14" s="55">
         <f ca="1">F12-3</f>
-        <v>45801</v>
+        <v>45820</v>
       </c>
       <c r="G14" s="56">
         <v>10</v>
@@ -18605,7 +17851,7 @@
       <c r="E15" s="54"/>
       <c r="F15" s="55">
         <f ca="1">F12+20</f>
-        <v>45824</v>
+        <v>45843</v>
       </c>
       <c r="G15" s="56">
         <v>1</v>
@@ -18850,7 +18096,7 @@
       </c>
       <c r="F16" s="55">
         <f ca="1">F12+6</f>
-        <v>45810</v>
+        <v>45829</v>
       </c>
       <c r="G16" s="56">
         <v>6</v>
@@ -19331,7 +18577,7 @@
       </c>
       <c r="F18" s="55">
         <f ca="1">F12+6</f>
-        <v>45810</v>
+        <v>45829</v>
       </c>
       <c r="G18" s="56">
         <v>13</v>
@@ -19576,7 +18822,7 @@
       </c>
       <c r="F19" s="55">
         <f ca="1">F18+2</f>
-        <v>45812</v>
+        <v>45831</v>
       </c>
       <c r="G19" s="56">
         <v>9</v>
@@ -19821,7 +19067,7 @@
       </c>
       <c r="F20" s="55">
         <f ca="1">F19+5</f>
-        <v>45817</v>
+        <v>45836</v>
       </c>
       <c r="G20" s="56">
         <v>11</v>
@@ -20064,7 +19310,7 @@
       <c r="E21" s="54"/>
       <c r="F21" s="55">
         <f ca="1">F20+2</f>
-        <v>45819</v>
+        <v>45838</v>
       </c>
       <c r="G21" s="56">
         <v>1</v>
@@ -20305,7 +19551,7 @@
       <c r="E22" s="54"/>
       <c r="F22" s="55">
         <f ca="1">F21+1</f>
-        <v>45820</v>
+        <v>45839</v>
       </c>
       <c r="G22" s="56">
         <v>24</v>
@@ -20784,7 +20030,7 @@
       <c r="E24" s="54"/>
       <c r="F24" s="55">
         <f ca="1">F12+15</f>
-        <v>45819</v>
+        <v>45838</v>
       </c>
       <c r="G24" s="56">
         <v>4</v>
@@ -21027,7 +20273,7 @@
       <c r="E25" s="54"/>
       <c r="F25" s="55">
         <f ca="1">F24+3</f>
-        <v>45822</v>
+        <v>45841</v>
       </c>
       <c r="G25" s="56">
         <v>14</v>
@@ -21270,7 +20516,7 @@
       <c r="E26" s="54"/>
       <c r="F26" s="55">
         <f ca="1">F25+15</f>
-        <v>45837</v>
+        <v>45856</v>
       </c>
       <c r="G26" s="56">
         <v>6</v>
@@ -21513,7 +20759,7 @@
       <c r="E27" s="54"/>
       <c r="F27" s="55">
         <f ca="1">F21+22</f>
-        <v>45841</v>
+        <v>45860</v>
       </c>
       <c r="G27" s="56">
         <v>3</v>
@@ -21756,7 +21002,7 @@
       <c r="E28" s="54"/>
       <c r="F28" s="55">
         <f ca="1">F16</f>
-        <v>45810</v>
+        <v>45829</v>
       </c>
       <c r="G28" s="56">
         <v>19</v>
@@ -22233,7 +21479,7 @@
       <c r="E30" s="54"/>
       <c r="F30" s="55">
         <f ca="1">F27+3</f>
-        <v>45844</v>
+        <v>45863</v>
       </c>
       <c r="G30" s="56">
         <v>15</v>
@@ -22474,7 +21720,7 @@
       <c r="E31" s="54"/>
       <c r="F31" s="55">
         <f ca="1">F30+14</f>
-        <v>45858</v>
+        <v>45877</v>
       </c>
       <c r="G31" s="56">
         <v>5</v>
@@ -22717,7 +21963,7 @@
       <c r="E32" s="54"/>
       <c r="F32" s="55">
         <f ca="1">F31+42</f>
-        <v>45900</v>
+        <v>45919</v>
       </c>
       <c r="G32" s="56">
         <v>1</v>
@@ -23757,39 +23003,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>AND($C10="Riesgo bajo",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>AND($C10="Riesgo alto",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>AND($C10="Según lo previsto",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>AND($C10="Riesgo medio",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23889,6 +23135,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -23906,15 +23161,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24212,28 +23458,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD6AD73-D703-40CF-AB8D-72E6A3921BEB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD6AD73-D703-40CF-AB8D-72E6A3921BEB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>